<commit_message>
fix losing formatting when inserting a range of values
</commit_message>
<xml_diff>
--- a/tests/sample.xlsx
+++ b/tests/sample.xlsx
@@ -47,9 +47,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0%"/>
+    <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -129,20 +130,28 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -166,39 +175,42 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.56"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2" t="n">
+      <c r="F1" s="3" t="n">
         <f aca="false">SUM(A5:D40)</f>
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>